<commit_message>
* Command line parameters are assigned first and then locked for further changes. * Re-factored classes related to internal data storage. * Added the possibility to use parameters in all the attributes in XML. * Minor changes in join layouts.
</commit_message>
<xml_diff>
--- a/tests/data/desired/numericaggregatedreport.xlsx
+++ b/tests/data/desired/numericaggregatedreport.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
-  <si>
-    <t>Field Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+  <si>
+    <t>Column Name</t>
   </si>
   <si>
     <t>ETYPE</t>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>M</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>NUM_INT</t>
@@ -213,12 +210,6 @@
       <c r="E3" t="n" s="3">
         <v>0.5</v>
       </c>
-      <c r="F3" t="s" s="3">
-        <v>10</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.0</v>
-      </c>
       <c r="H3" t="n">
         <v>4.0</v>
       </c>
@@ -228,7 +219,7 @@
     </row>
     <row r="4">
       <c r="B4" t="s" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -254,7 +245,7 @@
     </row>
     <row r="5">
       <c r="B5" t="s" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -280,7 +271,7 @@
     </row>
     <row r="6">
       <c r="B6" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -306,7 +297,7 @@
     </row>
     <row r="7">
       <c r="B7" t="s" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -332,7 +323,7 @@
     </row>
     <row r="8">
       <c r="B8" t="s" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -358,7 +349,7 @@
     </row>
     <row r="9">
       <c r="B9" t="s" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -387,7 +378,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" t="n">
         <v>2.0</v>
@@ -395,12 +386,6 @@
       <c r="E10" t="n" s="3">
         <v>0.6666666666666666</v>
       </c>
-      <c r="F10" t="s" s="3">
-        <v>10</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.0</v>
-      </c>
       <c r="H10" t="n">
         <v>3.0</v>
       </c>
@@ -410,10 +395,10 @@
     </row>
     <row r="11">
       <c r="B11" t="s" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" t="n">
         <v>3.0</v>
@@ -436,10 +421,10 @@
     </row>
     <row r="12">
       <c r="B12" t="s" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" t="n">
         <v>3.0</v>
@@ -462,10 +447,10 @@
     </row>
     <row r="13">
       <c r="B13" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" t="n">
         <v>3.0</v>
@@ -488,10 +473,10 @@
     </row>
     <row r="14">
       <c r="B14" t="s" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" t="n">
         <v>3.0</v>
@@ -514,10 +499,10 @@
     </row>
     <row r="15">
       <c r="B15" t="s" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" t="n">
         <v>3.0</v>
@@ -540,10 +525,10 @@
     </row>
     <row r="16">
       <c r="B16" t="s" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" t="n">
         <v>3.0</v>

</xml_diff>

<commit_message>
* Do not show total value in aggregated report for non-numeric columns.
</commit_message>
<xml_diff>
--- a/tests/data/desired/numericaggregatedreport.xlsx
+++ b/tests/data/desired/numericaggregatedreport.xlsx
@@ -213,9 +213,6 @@
       <c r="H3" t="n">
         <v>4.0</v>
       </c>
-      <c r="I3" t="n">
-        <v>0.0</v>
-      </c>
     </row>
     <row r="4">
       <c r="B4" t="s" s="2">
@@ -388,9 +385,6 @@
       </c>
       <c r="H10" t="n">
         <v>3.0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.0</v>
       </c>
     </row>
     <row r="11">

</xml_diff>